<commit_message>
ajustando erros de informação
</commit_message>
<xml_diff>
--- a/casos_por_ano.xlsx
+++ b/casos_por_ano.xlsx
@@ -508,10 +508,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>320</v>
+        <v>259</v>
       </c>
       <c r="D5" t="n">
-        <v>19.54</v>
+        <v>15.81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
versão 2.1 adicionado anos de 2018, 2019 e 2020
</commit_message>
<xml_diff>
--- a/casos_por_ano.xlsx
+++ b/casos_por_ano.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,14 +456,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>667</v>
+        <v>1871</v>
       </c>
       <c r="D2" t="n">
-        <v>11.49</v>
+        <v>32.23</v>
       </c>
     </row>
     <row r="3">
@@ -472,14 +472,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>541</v>
+        <v>1260</v>
       </c>
       <c r="D3" t="n">
-        <v>9.32</v>
+        <v>21.71</v>
       </c>
     </row>
     <row r="4">
@@ -488,14 +488,14 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>522</v>
+        <v>682</v>
       </c>
       <c r="D4" t="n">
-        <v>8.99</v>
+        <v>11.75</v>
       </c>
     </row>
     <row r="5">
@@ -504,13 +504,61 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>667</v>
+      </c>
+      <c r="D5" t="n">
+        <v>11.49</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>541</v>
+      </c>
+      <c r="D6" t="n">
+        <v>9.32</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>522</v>
+      </c>
+      <c r="D7" t="n">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>2024</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C8" t="n">
         <v>258</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D8" t="n">
         <v>4.44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
versão 2.7  salvando arquivos em xlsx
</commit_message>
<xml_diff>
--- a/casos_por_ano.xlsx
+++ b/casos_por_ano.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>